<commit_message>
added primary auditors and secondary auditors for JWA batches. plus scheduled qc sesstion for the batch. primary auditors for some Java, .net, and sales force were added too
</commit_message>
<xml_diff>
--- a/TrackPTO/Dummy QC Schedule Copy (1).xlsx
+++ b/TrackPTO/Dummy QC Schedule Copy (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahme\Documents\UiPath\TrackPTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B58928D-969C-45A0-AE4C-FEA453287809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC1D624-8EE8-453C-8A09-B73F7EF9AFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="14400" windowHeight="8273" tabRatio="605" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="605" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scheduling Rules" sheetId="77" r:id="rId1"/>
@@ -2000,7 +2000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DD456-57E5-4742-8C33-0141C486BDCA}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -3422,8 +3422,8 @@
   </sheetPr>
   <dimension ref="A1:O981"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12581,21 +12581,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010035320A12CFF460459638DE9B86DD9357" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f11676696cc246df58d12072c86cf252">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5789d6d3-4852-43c5-9082-41a0df76b368" xmlns:ns4="f28bebd9-3202-45a0-b989-5e5ae93a89b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ea6d730d764c2aef8b02e40be4db643" ns3:_="" ns4:_="">
     <xsd:import namespace="5789d6d3-4852-43c5-9082-41a0df76b368"/>
@@ -12818,24 +12803,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F62D5D-402C-4D37-8B1B-B293D3FE1710}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E74CAD0-3F93-445C-B91B-678382B98543}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12852,4 +12835,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81B5B8A7-0BC9-4D7F-8134-9CC058C7B2A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F62D5D-402C-4D37-8B1B-B293D3FE1710}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>